<commit_message>
se actualizo el thesaure
</commit_message>
<xml_diff>
--- a/02-Sesion/Thesaurus.xlsx
+++ b/02-Sesion/Thesaurus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carolina\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC69F6A3-3465-4FE0-BDFD-C399ED7436C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAFAC02-7A4E-4A43-8955-2F1ECB64CF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CBF535E4-71E5-47C2-9BF5-65E8EF8C5F03}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="158">
   <si>
     <t>Término o Frase</t>
   </si>
@@ -397,9 +397,6 @@
     <t>que es "Arquitectura de software"</t>
   </si>
   <si>
-    <t>6/26/2017</t>
-  </si>
-  <si>
     <t>https://www.scielo.cl/scielo.php?pid=S0718-33052018000300376&amp;script=sci_arttext</t>
   </si>
   <si>
@@ -531,6 +528,16 @@
   </si>
   <si>
     <t>ujaen.es</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Antonio-Mana/publication/228673463_Integrando_la_Ingenieria_de_Seguridad_en_un_Proceso_de_Ingenieria_Software/links/0046351ac647386db4000000/Integrando-la-Ingenieria-de-Seguridad-en-un-Proceso-de-Ingenieria-Software.pdf</t>
+  </si>
+  <si>
+    <t>Integrando la Ingeniería de Seguridad en un 
+ Proceso de Ingeniería Software</t>
+  </si>
+  <si>
+    <t>patrones de diseño software</t>
   </si>
 </sst>
 </file>
@@ -540,7 +547,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -597,8 +604,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,19 +652,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,6 +660,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA9D08E"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -760,7 +775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -821,9 +836,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -833,9 +845,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -843,9 +852,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -869,35 +875,47 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1218,8 +1236,8 @@
   <dimension ref="A1:Z45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="84" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1425,7 +1443,7 @@
       <c r="F7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="43" t="s">
         <v>34</v>
       </c>
       <c r="H7" s="19">
@@ -1503,14 +1521,16 @@
       <c r="C10" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="21">
+        <v>45610</v>
+      </c>
       <c r="E10" s="23" t="s">
         <v>44</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="43" t="s">
         <v>46</v>
       </c>
       <c r="H10" s="22">
@@ -1646,14 +1666,16 @@
       <c r="C15" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="21"/>
+      <c r="D15" s="21">
+        <v>45609</v>
+      </c>
       <c r="E15" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="43" t="s">
         <v>62</v>
       </c>
       <c r="H15" s="22">
@@ -1673,14 +1695,16 @@
       <c r="C16" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="21">
+        <v>45609</v>
+      </c>
       <c r="E16" s="23" t="s">
         <v>64</v>
       </c>
       <c r="F16" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="43" t="s">
         <v>65</v>
       </c>
       <c r="H16" s="22">
@@ -1700,14 +1724,16 @@
       <c r="C17" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="21">
+        <v>45610</v>
+      </c>
       <c r="E17" s="23" t="s">
         <v>73</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="43" t="s">
         <v>74</v>
       </c>
       <c r="H17" s="22">
@@ -1756,14 +1782,16 @@
       <c r="C19" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="21"/>
+      <c r="D19" s="21">
+        <v>45609</v>
+      </c>
       <c r="E19" s="23" t="s">
         <v>79</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="43" t="s">
         <v>81</v>
       </c>
       <c r="H19" s="22">
@@ -1812,14 +1840,16 @@
       <c r="C21" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="21"/>
+      <c r="D21" s="21">
+        <v>45609</v>
+      </c>
       <c r="E21" s="23" t="s">
         <v>88</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="43" t="s">
         <v>89</v>
       </c>
       <c r="H21" s="22">
@@ -1828,23 +1858,23 @@
       <c r="I21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="47"/>
-      <c r="V21" s="47"/>
-      <c r="W21" s="47"/>
-      <c r="X21" s="47"/>
-      <c r="Y21" s="47"/>
-      <c r="Z21" s="47"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="40"/>
+      <c r="W21" s="40"/>
+      <c r="X21" s="40"/>
+      <c r="Y21" s="40"/>
+      <c r="Z21" s="40"/>
     </row>
     <row r="22" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="20">
@@ -1856,14 +1886,16 @@
       <c r="C22" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="21"/>
+      <c r="D22" s="21">
+        <v>45610</v>
+      </c>
       <c r="E22" s="23" t="s">
         <v>91</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="43" t="s">
         <v>92</v>
       </c>
       <c r="H22" s="22">
@@ -1883,14 +1915,16 @@
       <c r="C23" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="21"/>
+      <c r="D23" s="21">
+        <v>45611</v>
+      </c>
       <c r="E23" s="23" t="s">
         <v>95</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="43" t="s">
         <v>97</v>
       </c>
       <c r="H23" s="22">
@@ -1939,14 +1973,16 @@
       <c r="C25" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="21"/>
+      <c r="D25" s="21">
+        <v>45611</v>
+      </c>
       <c r="E25" s="23" t="s">
         <v>102</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="G25" s="24" t="s">
+      <c r="G25" s="45" t="s">
         <v>104</v>
       </c>
       <c r="H25" s="22">
@@ -1957,78 +1993,82 @@
       </c>
     </row>
     <row r="26" spans="1:26" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="26">
+      <c r="A26" s="25">
         <v>25</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29" t="s">
+      <c r="D26" s="21">
+        <v>45611</v>
+      </c>
+      <c r="E26" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="F26" s="27" t="s">
+      <c r="F26" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="G26" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="28">
         <v>4830</v>
       </c>
-      <c r="I26" s="27" t="s">
+      <c r="I26" s="26" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="79.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="50">
+      <c r="A27" s="42">
         <v>26</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="40"/>
-      <c r="E27" s="29" t="s">
+      <c r="D27" s="21">
+        <v>45611</v>
+      </c>
+      <c r="E27" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="36" t="s">
         <v>111</v>
       </c>
       <c r="G27" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="H27" s="39">
+      <c r="H27" s="36">
         <v>169</v>
       </c>
-      <c r="I27" s="41" t="s">
+      <c r="I27" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="J27" s="37"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="25"/>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="25"/>
-      <c r="U27" s="25"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="25"/>
-      <c r="X27" s="25"/>
-      <c r="Y27" s="25"/>
-      <c r="Z27" s="25"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="24"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="24"/>
+      <c r="T27" s="24"/>
+      <c r="U27" s="24"/>
+      <c r="V27" s="24"/>
+      <c r="W27" s="24"/>
+      <c r="X27" s="24"/>
+      <c r="Y27" s="24"/>
+      <c r="Z27" s="24"/>
     </row>
     <row r="28" spans="1:26" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="50">
+      <c r="A28" s="42">
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -2037,88 +2077,92 @@
       <c r="C28" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="21">
+        <v>45611</v>
+      </c>
+      <c r="E28" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="F28" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="G28" s="43" t="s">
         <v>116</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>117</v>
       </c>
       <c r="H28" s="15">
         <v>20300</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="J28" s="42"/>
-      <c r="K28" s="35"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="25"/>
-      <c r="T28" s="25"/>
-      <c r="U28" s="25"/>
-      <c r="V28" s="25"/>
-      <c r="W28" s="25"/>
-      <c r="X28" s="25"/>
-      <c r="Y28" s="25"/>
-      <c r="Z28" s="25"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="24"/>
+      <c r="T28" s="24"/>
+      <c r="U28" s="24"/>
+      <c r="V28" s="24"/>
+      <c r="W28" s="24"/>
+      <c r="X28" s="24"/>
+      <c r="Y28" s="24"/>
+      <c r="Z28" s="24"/>
     </row>
     <row r="29" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="50">
+      <c r="A29" s="42">
         <v>28</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="21">
+        <v>45612</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="H29" s="30">
+        <v>745000</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="35">
+        <v>29</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" s="21">
+        <v>45612</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="43" t="s">
         <v>121</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="32"/>
-      <c r="E29" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="F29" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="48" t="s">
-        <v>119</v>
-      </c>
-      <c r="H29" s="33">
-        <v>745000</v>
-      </c>
-      <c r="I29" s="31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="38">
-        <v>29</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>122</v>
       </c>
       <c r="H30" s="22">
         <v>167000</v>
@@ -2128,24 +2172,26 @@
       </c>
     </row>
     <row r="31" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="38">
+      <c r="A31" s="35">
         <v>30</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="21">
+        <v>45612</v>
+      </c>
+      <c r="E31" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="23" t="s">
+      <c r="F31" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" s="43" t="s">
         <v>126</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="G31" s="24" t="s">
-        <v>127</v>
       </c>
       <c r="H31" s="22">
         <v>167000</v>
@@ -2155,24 +2201,26 @@
       </c>
     </row>
     <row r="32" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="38">
+      <c r="A32" s="35">
         <v>31</v>
       </c>
-      <c r="B32" s="49" t="s">
-        <v>134</v>
+      <c r="B32" s="41" t="s">
+        <v>133</v>
       </c>
       <c r="C32" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="21">
+        <v>45612</v>
+      </c>
+      <c r="E32" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="23" t="s">
-        <v>133</v>
-      </c>
       <c r="F32" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="G32" s="24" t="s">
         <v>130</v>
+      </c>
+      <c r="G32" s="43" t="s">
+        <v>129</v>
       </c>
       <c r="H32" s="22">
         <v>182000</v>
@@ -2182,24 +2230,26 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="38">
+      <c r="A33" s="35">
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D33" s="21"/>
+        <v>131</v>
+      </c>
+      <c r="D33" s="21">
+        <v>45612</v>
+      </c>
       <c r="E33" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G33" s="24" t="s">
-        <v>135</v>
+      <c r="G33" s="43" t="s">
+        <v>134</v>
       </c>
       <c r="H33" s="22">
         <v>182000</v>
@@ -2209,24 +2259,26 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="38">
+      <c r="A34" s="35">
         <v>33</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D34" s="21"/>
+        <v>131</v>
+      </c>
+      <c r="D34" s="21">
+        <v>45612</v>
+      </c>
       <c r="E34" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F34" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="G34" s="24" t="s">
-        <v>138</v>
+      <c r="G34" s="43" t="s">
+        <v>137</v>
       </c>
       <c r="H34" s="22">
         <v>182000</v>
@@ -2236,24 +2288,26 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="38">
+      <c r="A35" s="35">
         <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D35" s="21"/>
+        <v>144</v>
+      </c>
+      <c r="D35" s="21">
+        <v>45612</v>
+      </c>
       <c r="E35" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="G35" s="24" t="s">
         <v>142</v>
+      </c>
+      <c r="G35" s="43" t="s">
+        <v>141</v>
       </c>
       <c r="H35" s="22">
         <v>24500</v>
@@ -2263,24 +2317,26 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="38">
+      <c r="A36" s="35">
         <v>35</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="21">
+        <v>45612</v>
+      </c>
+      <c r="E36" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="23" t="s">
+      <c r="F36" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" s="43" t="s">
         <v>146</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>147</v>
       </c>
       <c r="H36" s="22">
         <v>24500</v>
@@ -2290,24 +2346,26 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="38">
+      <c r="A37" s="35">
         <v>36</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>87</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="D37" s="21"/>
+        <v>151</v>
+      </c>
+      <c r="D37" s="21">
+        <v>45612</v>
+      </c>
       <c r="E37" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G37" s="43" t="s">
         <v>149</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>150</v>
       </c>
       <c r="H37" s="22">
         <v>29300</v>
@@ -2317,24 +2375,26 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="38">
+      <c r="A38" s="35">
         <v>37</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>87</v>
       </c>
       <c r="C38" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" s="21">
+        <v>45612</v>
+      </c>
+      <c r="E38" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" s="43" t="s">
         <v>152</v>
-      </c>
-      <c r="D38" s="21"/>
-      <c r="E38" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>153</v>
       </c>
       <c r="H38" s="22">
         <v>29300</v>
@@ -2343,16 +2403,34 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="3"/>
+    <row r="39" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="35">
+        <v>37</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="21">
+        <v>45612</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F39" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="G39" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="H39" s="50">
+        <v>126000</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
@@ -2452,8 +2530,9 @@
     <hyperlink ref="E36" r:id="rId35" xr:uid="{4B0E6557-84C8-4DDC-A9A1-10657E878E37}"/>
     <hyperlink ref="E37" r:id="rId36" xr:uid="{7338AAFB-CD5D-47CC-93F5-D7E5B4B652CC}"/>
     <hyperlink ref="E38" r:id="rId37" xr:uid="{88E9A0C1-DE5D-4A2A-9F2C-B475E4C71F42}"/>
+    <hyperlink ref="E39" r:id="rId38" display="https://www.researchgate.net/profile/Antonio-Mana/publication/228673463_Integrando_la_Ingenieria_de_Seguridad_en_un_Proceso_de_Ingenieria_Software/links/0046351ac647386db4000000/Integrando-la-Ingenieria-de-Seguridad-en-un-Proceso-de-Ingenieria-Software.pdf" xr:uid="{F24D655F-1E78-4EC9-A248-96B259F031C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>